<commit_message>
calc toxicity at diff lengths
</commit_message>
<xml_diff>
--- a/toxicity_detection/mitigation/frequency_of_identity_lemmas.xlsx
+++ b/toxicity_detection/mitigation/frequency_of_identity_lemmas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,27 +446,37 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>nontoxic_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>total_count</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>toxic_pct</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>nontoxic_pct</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>total_pct</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>difference</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>abs_difference</t>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>tox_total_diff</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>tox_total_abs_diff</t>
         </is>
       </c>
     </row>
@@ -483,18 +493,24 @@
         <v>16</v>
       </c>
       <c r="D2" t="n">
+        <v>57</v>
+      </c>
+      <c r="E2" t="n">
         <v>73</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>4.597701149425287</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
+        <v>2.496714848883049</v>
+      </c>
+      <c r="H2" t="n">
         <v>2.774610414291144</v>
       </c>
-      <c r="G2" t="n">
+      <c r="I2" t="n">
         <v>1.823090735134143</v>
       </c>
-      <c r="H2" t="n">
+      <c r="J2" t="n">
         <v>1.823090735134143</v>
       </c>
     </row>
@@ -511,18 +527,24 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
+        <v>26</v>
+      </c>
+      <c r="E3" t="n">
         <v>33</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>2.011494252873563</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
+        <v>1.138852387209812</v>
+      </c>
+      <c r="H3" t="n">
         <v>1.254275940706955</v>
       </c>
-      <c r="G3" t="n">
+      <c r="I3" t="n">
         <v>0.7572183121666078</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.7572183121666078</v>
       </c>
     </row>
@@ -539,18 +561,24 @@
         <v>1</v>
       </c>
       <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G4" t="n">
+      <c r="I4" t="n">
         <v>0.2493479599994757</v>
       </c>
-      <c r="H4" t="n">
+      <c r="J4" t="n">
         <v>0.2493479599994757</v>
       </c>
     </row>
@@ -567,18 +595,24 @@
         <v>1</v>
       </c>
       <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
         <v>1</v>
       </c>
-      <c r="E5" t="n">
+      <c r="F5" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G5" t="n">
+      <c r="I5" t="n">
         <v>0.2493479599994757</v>
       </c>
-      <c r="H5" t="n">
+      <c r="J5" t="n">
         <v>0.2493479599994757</v>
       </c>
     </row>
@@ -595,18 +629,24 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="n">
+      <c r="F6" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G6" t="n">
+      <c r="I6" t="n">
         <v>0.2493479599994757</v>
       </c>
-      <c r="H6" t="n">
+      <c r="J6" t="n">
         <v>0.2493479599994757</v>
       </c>
     </row>
@@ -623,18 +663,24 @@
         <v>1</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>1</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G7" t="n">
+      <c r="I7" t="n">
         <v>0.2493479599994757</v>
       </c>
-      <c r="H7" t="n">
+      <c r="J7" t="n">
         <v>0.2493479599994757</v>
       </c>
     </row>
@@ -651,18 +697,24 @@
         <v>1</v>
       </c>
       <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G8" t="n">
+      <c r="I8" t="n">
         <v>0.2493479599994757</v>
       </c>
-      <c r="H8" t="n">
+      <c r="J8" t="n">
         <v>0.2493479599994757</v>
       </c>
     </row>
@@ -679,18 +731,24 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="n">
         <v>2</v>
       </c>
-      <c r="E9" t="n">
+      <c r="F9" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
+        <v>0.04380201489268506</v>
+      </c>
+      <c r="H9" t="n">
         <v>0.07601672367920942</v>
       </c>
-      <c r="G9" t="n">
+      <c r="I9" t="n">
         <v>0.211339598159871</v>
       </c>
-      <c r="H9" t="n">
+      <c r="J9" t="n">
         <v>0.211339598159871</v>
       </c>
     </row>
@@ -707,18 +765,24 @@
         <v>1</v>
       </c>
       <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
         <v>3</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
+        <v>0.08760402978537013</v>
+      </c>
+      <c r="H10" t="n">
         <v>0.1140250855188141</v>
       </c>
-      <c r="G10" t="n">
+      <c r="I10" t="n">
         <v>0.1733312363202663</v>
       </c>
-      <c r="H10" t="n">
+      <c r="J10" t="n">
         <v>0.1733312363202663</v>
       </c>
     </row>
@@ -735,18 +799,24 @@
         <v>2</v>
       </c>
       <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
         <v>11</v>
       </c>
-      <c r="E11" t="n">
+      <c r="F11" t="n">
         <v>0.5747126436781609</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
+        <v>0.3942181340341656</v>
+      </c>
+      <c r="H11" t="n">
         <v>0.4180919802356519</v>
       </c>
-      <c r="G11" t="n">
+      <c r="I11" t="n">
         <v>0.156620663442509</v>
       </c>
-      <c r="H11" t="n">
+      <c r="J11" t="n">
         <v>0.156620663442509</v>
       </c>
     </row>
@@ -763,18 +833,24 @@
         <v>1</v>
       </c>
       <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="n">
         <v>6</v>
       </c>
-      <c r="E12" t="n">
+      <c r="F12" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
+        <v>0.2190100744634253</v>
+      </c>
+      <c r="H12" t="n">
         <v>0.2280501710376283</v>
       </c>
-      <c r="G12" t="n">
+      <c r="I12" t="n">
         <v>0.05930615080145216</v>
       </c>
-      <c r="H12" t="n">
+      <c r="J12" t="n">
         <v>0.05930615080145216</v>
       </c>
     </row>
@@ -791,18 +867,24 @@
         <v>1</v>
       </c>
       <c r="D13" t="n">
+        <v>5</v>
+      </c>
+      <c r="E13" t="n">
         <v>6</v>
       </c>
-      <c r="E13" t="n">
+      <c r="F13" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
+        <v>0.2190100744634253</v>
+      </c>
+      <c r="H13" t="n">
         <v>0.2280501710376283</v>
       </c>
-      <c r="G13" t="n">
+      <c r="I13" t="n">
         <v>0.05930615080145216</v>
       </c>
-      <c r="H13" t="n">
+      <c r="J13" t="n">
         <v>0.05930615080145216</v>
       </c>
     </row>
@@ -833,6 +915,12 @@
       <c r="H14" t="n">
         <v>0</v>
       </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -861,6 +949,12 @@
       <c r="H15" t="n">
         <v>0</v>
       </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -889,6 +983,12 @@
       <c r="H16" t="n">
         <v>0</v>
       </c>
+      <c r="I16" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -917,6 +1017,12 @@
       <c r="H17" t="n">
         <v>0</v>
       </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -945,6 +1051,12 @@
       <c r="H18" t="n">
         <v>0</v>
       </c>
+      <c r="I18" t="n">
+        <v>0</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -973,6 +1085,12 @@
       <c r="H19" t="n">
         <v>0</v>
       </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1001,6 +1119,12 @@
       <c r="H20" t="n">
         <v>0</v>
       </c>
+      <c r="I20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1029,6 +1153,12 @@
       <c r="H21" t="n">
         <v>0</v>
       </c>
+      <c r="I21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1057,6 +1187,12 @@
       <c r="H22" t="n">
         <v>0</v>
       </c>
+      <c r="I22" t="n">
+        <v>0</v>
+      </c>
+      <c r="J22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1085,6 +1221,12 @@
       <c r="H23" t="n">
         <v>0</v>
       </c>
+      <c r="I23" t="n">
+        <v>0</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1113,6 +1255,12 @@
       <c r="H24" t="n">
         <v>0</v>
       </c>
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1141,6 +1289,12 @@
       <c r="H25" t="n">
         <v>0</v>
       </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1169,6 +1323,12 @@
       <c r="H26" t="n">
         <v>0</v>
       </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -1197,6 +1357,12 @@
       <c r="H27" t="n">
         <v>0</v>
       </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -1225,6 +1391,12 @@
       <c r="H28" t="n">
         <v>0</v>
       </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -1253,6 +1425,12 @@
       <c r="H29" t="n">
         <v>0</v>
       </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -1281,6 +1459,12 @@
       <c r="H30" t="n">
         <v>0</v>
       </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -1309,6 +1493,12 @@
       <c r="H31" t="n">
         <v>0</v>
       </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -1337,6 +1527,12 @@
       <c r="H32" t="n">
         <v>0</v>
       </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -1365,6 +1561,12 @@
       <c r="H33" t="n">
         <v>0</v>
       </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -1393,6 +1595,12 @@
       <c r="H34" t="n">
         <v>0</v>
       </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -1421,6 +1629,12 @@
       <c r="H35" t="n">
         <v>0</v>
       </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -1449,6 +1663,12 @@
       <c r="H36" t="n">
         <v>0</v>
       </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -1477,6 +1697,12 @@
       <c r="H37" t="n">
         <v>0</v>
       </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -1505,6 +1731,12 @@
       <c r="H38" t="n">
         <v>0</v>
       </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1519,18 +1751,24 @@
         <v>1</v>
       </c>
       <c r="D39" t="n">
+        <v>7</v>
+      </c>
+      <c r="E39" t="n">
         <v>8</v>
       </c>
-      <c r="E39" t="n">
+      <c r="F39" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
+        <v>0.3066141042487955</v>
+      </c>
+      <c r="H39" t="n">
         <v>0.3040668947168377</v>
       </c>
-      <c r="G39" t="n">
+      <c r="I39" t="n">
         <v>-0.01671057287775723</v>
       </c>
-      <c r="H39" t="n">
+      <c r="J39" t="n">
         <v>0.01671057287775723</v>
       </c>
     </row>
@@ -1550,15 +1788,21 @@
         <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.04380201489268506</v>
+      </c>
+      <c r="H40" t="n">
         <v>0.03800836183960471</v>
       </c>
-      <c r="G40" t="n">
+      <c r="I40" t="n">
         <v>-0.03800836183960471</v>
       </c>
-      <c r="H40" t="n">
+      <c r="J40" t="n">
         <v>0.03800836183960471</v>
       </c>
     </row>
@@ -1578,15 +1822,21 @@
         <v>2</v>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.08760402978537013</v>
+      </c>
+      <c r="H41" t="n">
         <v>0.07601672367920942</v>
       </c>
-      <c r="G41" t="n">
+      <c r="I41" t="n">
         <v>-0.07601672367920942</v>
       </c>
-      <c r="H41" t="n">
+      <c r="J41" t="n">
         <v>0.07601672367920942</v>
       </c>
     </row>
@@ -1606,15 +1856,21 @@
         <v>3</v>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.1314060446780552</v>
+      </c>
+      <c r="H42" t="n">
         <v>0.1140250855188141</v>
       </c>
-      <c r="G42" t="n">
+      <c r="I42" t="n">
         <v>-0.1140250855188141</v>
       </c>
-      <c r="H42" t="n">
+      <c r="J42" t="n">
         <v>0.1140250855188141</v>
       </c>
     </row>
@@ -1631,18 +1887,24 @@
         <v>1</v>
       </c>
       <c r="D43" t="n">
+        <v>10</v>
+      </c>
+      <c r="E43" t="n">
         <v>11</v>
       </c>
-      <c r="E43" t="n">
+      <c r="F43" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
+        <v>0.4380201489268506</v>
+      </c>
+      <c r="H43" t="n">
         <v>0.4180919802356519</v>
       </c>
-      <c r="G43" t="n">
+      <c r="I43" t="n">
         <v>-0.1307356583965714</v>
       </c>
-      <c r="H43" t="n">
+      <c r="J43" t="n">
         <v>0.1307356583965714</v>
       </c>
     </row>
@@ -1659,18 +1921,24 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
+        <v>11</v>
+      </c>
+      <c r="E44" t="n">
         <v>12</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>0.2873563218390804</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
+        <v>0.4818221638195357</v>
+      </c>
+      <c r="H44" t="n">
         <v>0.4561003420752566</v>
       </c>
-      <c r="G44" t="n">
+      <c r="I44" t="n">
         <v>-0.1687440202361761</v>
       </c>
-      <c r="H44" t="n">
+      <c r="J44" t="n">
         <v>0.1687440202361761</v>
       </c>
     </row>
@@ -1690,15 +1958,21 @@
         <v>5</v>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.2190100744634253</v>
+      </c>
+      <c r="H45" t="n">
         <v>0.1900418091980235</v>
       </c>
-      <c r="G45" t="n">
+      <c r="I45" t="n">
         <v>-0.1900418091980235</v>
       </c>
-      <c r="H45" t="n">
+      <c r="J45" t="n">
         <v>0.1900418091980235</v>
       </c>
     </row>
@@ -1718,15 +1992,21 @@
         <v>5</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0.2190100744634253</v>
+      </c>
+      <c r="H46" t="n">
         <v>0.1900418091980235</v>
       </c>
-      <c r="G46" t="n">
+      <c r="I46" t="n">
         <v>-0.1900418091980235</v>
       </c>
-      <c r="H46" t="n">
+      <c r="J46" t="n">
         <v>0.1900418091980235</v>
       </c>
     </row>

</xml_diff>